<commit_message>
Copia antes de añadir evolucion part number
</commit_message>
<xml_diff>
--- a/xls/350.xlsx
+++ b/xls/350.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NG75BA7\Desktop\412\programaPython\peticiones\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" firstSheet="4" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="1000" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Componentes" sheetId="1" r:id="rId1"/>
@@ -20,15 +15,17 @@
     <sheet name="AREA_APT3" sheetId="5" r:id="rId6"/>
     <sheet name="AREA_APT4" sheetId="6" r:id="rId7"/>
     <sheet name="AREA_APT5" sheetId="7" r:id="rId8"/>
-    <sheet name="DESVIACION_APT1" sheetId="8" r:id="rId9"/>
-    <sheet name="DESVIACION_APT2" sheetId="9" r:id="rId10"/>
-    <sheet name="DESVIACION_APT3" sheetId="10" r:id="rId11"/>
-    <sheet name="DESVIACION_APT4" sheetId="11" r:id="rId12"/>
-    <sheet name="DESVIACION_APT5" sheetId="12" r:id="rId13"/>
-    <sheet name="PIEZA" sheetId="13" r:id="rId14"/>
-    <sheet name="SGM" sheetId="14" r:id="rId15"/>
+    <sheet name="AREA_APT9" sheetId="16" r:id="rId9"/>
+    <sheet name="DESVIACION_APT1" sheetId="8" r:id="rId10"/>
+    <sheet name="DESVIACION_APT2" sheetId="9" r:id="rId11"/>
+    <sheet name="DESVIACION_APT3" sheetId="10" r:id="rId12"/>
+    <sheet name="DESVIACION_APT4" sheetId="11" r:id="rId13"/>
+    <sheet name="DESVIACION_APT5" sheetId="12" r:id="rId14"/>
+    <sheet name="DESVIACION_APT9" sheetId="17" r:id="rId15"/>
+    <sheet name="PIEZA" sheetId="13" r:id="rId16"/>
+    <sheet name="SGM" sheetId="14" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -38,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="166">
   <si>
     <t>Componente</t>
   </si>
@@ -894,7 +891,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1111,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,55 +1124,82 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>165</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>28</v>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>101</v>
+      </c>
+      <c r="B10" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>101</v>
+      <c r="A11" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1190,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,51 +1229,87 @@
       <c r="A1" t="s">
         <v>13</v>
       </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1268,7 +1328,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,46 +1345,63 @@
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1340,10 +1417,102 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1025" width="10.7109375"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,53 +1531,70 @@
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="O4" s="4"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="O6" s="4"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1422,7 +1608,108 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -1460,12 +1747,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1915,7 +2202,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1990,7 +2277,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection sqref="A1:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2286,86 +2573,120 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1025" width="10.7109375"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>164</v>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Copia antes de añadir apt9
</commit_message>
<xml_diff>
--- a/xls/350.xlsx
+++ b/xls/350.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="1000" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Componentes" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="166">
   <si>
     <t>Componente</t>
   </si>
@@ -891,7 +891,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1108,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,79 +1126,57 @@
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>165</v>
-      </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>101</v>
       </c>
-      <c r="B10" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B11" s="2" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1217,7 +1195,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection sqref="A1:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,87 +1207,57 @@
       <c r="A1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B11" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1328,7 +1276,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,63 +1293,46 @@
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1420,7 +1351,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,63 +1368,46 @@
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1512,7 +1426,9 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+      <pane xSplit="16410" topLeftCell="E1"/>
+      <selection activeCell="J9" sqref="J9"/>
+      <selection pane="topRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,70 +1447,53 @@
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="B2" s="3"/>
       <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="B3" s="3"/>
       <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="B4" s="3"/>
       <c r="O4" s="4"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="B5" s="3"/>
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="B6" s="3"/>
       <c r="O6" s="4"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="B7" s="3"/>
       <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="B8" s="3"/>
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" s="3" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1610,102 +1509,71 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B11"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>101</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1751,7 +1619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>